<commit_message>
adding of resulting screen and change of excel
</commit_message>
<xml_diff>
--- a/Config/Excel/LevelInfoData.xlsx
+++ b/Config/Excel/LevelInfoData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\Biggerlab_Ryan_Git\the-janitor-simulator\Config\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\blcode\the-janitor-simulator\Config\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD41A57-8AAE-44C1-A716-EDD165D55176}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9B1EA7-B2E9-447B-8D9A-34E1C01F792E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="900" windowWidth="25110" windowHeight="12615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LevelInfo" sheetId="1" r:id="rId1"/>
@@ -109,18 +109,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Class</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PlayerGround</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>sdsads</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>The enemy from the east declared war to the republic few days ago. Although the government promised that Combo city would not be occupied, the city meets the invaders soon after the rout of the troops at the front line.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -145,17 +137,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>100,60,21</t>
-  </si>
-  <si>
-    <t>100,60,22</t>
+    <t>HallWay</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ClassRoom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>80,50,30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100,70,20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +167,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -193,7 +203,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -205,6 +215,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -483,21 +496,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.375" customWidth="1"/>
-    <col min="2" max="3" width="34.375" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="3" width="34.33203125" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
-    <col min="5" max="5" width="29.125" customWidth="1"/>
-    <col min="6" max="7" width="28.875" customWidth="1"/>
-    <col min="8" max="8" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" customWidth="1"/>
+    <col min="6" max="7" width="28.88671875" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -546,10 +559,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -572,36 +585,36 @@
         <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>10001</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>18</v>
@@ -610,24 +623,24 @@
         <v>10002</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="95.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>10002</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>26</v>
+      <c r="B7" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>19</v>
@@ -635,16 +648,16 @@
       <c r="G7" s="1">
         <v>10003</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="122.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="122.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>10003</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
+      <c r="B8" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>24</v>
@@ -653,7 +666,7 @@
         <v>16</v>
       </c>
       <c r="E8">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>20</v>
@@ -661,64 +674,64 @@
       <c r="G8" s="1">
         <v>10001</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>